<commit_message>
feat: novos campos para envio de pedidos da Estante Virtual
</commit_message>
<xml_diff>
--- a/public/upload-file/template/Envio de pedidos da Estante Virtual.xlsx
+++ b/public/upload-file/template/Envio de pedidos da Estante Virtual.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LowCost\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LowCost\Projetos\B1Sistema-PDOCRUD\resources\react-app\public\upload-file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8184C8CA-479F-4EB9-9A49-D0FAAD8D544E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1665DD3D-F7A6-484B-BC60-9811181F12D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="1710" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Data de pagamento</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Metodo de pagamento</t>
+  </si>
+  <si>
+    <t>Data para envio</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,9 +504,10 @@
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,13 +598,17 @@
       <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>